<commit_message>
Fim dos teste, falta terminar o relatorio.
</commit_message>
<xml_diff>
--- a/Avaliação/Tabelas.xlsx
+++ b/Avaliação/Tabelas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="415" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="832" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3244" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3364" uniqueCount="139">
   <si>
     <t>ENPC – Bases Desbalanceadas</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t>0.18</t>
+  </si>
+  <si>
+    <t>0.34</t>
   </si>
 </sst>
 </file>
@@ -588,8 +591,8 @@
   </sheetPr>
   <dimension ref="A1:AA258"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A220" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E250" activeCellId="0" pane="topLeft" sqref="E250"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D220" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="E256" activeCellId="0" pane="topLeft" sqref="E256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11967,7 +11970,7 @@
       </c>
       <c r="AA245" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="246">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="246">
       <c r="C246" s="7" t="n">
         <v>1</v>
       </c>
@@ -11975,34 +11978,34 @@
         <v>81</v>
       </c>
       <c r="E246" s="7" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="F246" s="7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G246" s="7" t="s">
         <v>84</v>
       </c>
       <c r="H246" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="I246" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J246" s="7" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="K246" s="7" t="s">
         <v>14</v>
       </c>
       <c r="L246" s="7" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="M246" s="7" t="s">
         <v>61</v>
       </c>
       <c r="N246" s="7" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P246" s="7" t="n">
         <v>1</v>
@@ -12010,18 +12013,38 @@
       <c r="Q246" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="R246" s="7"/>
-      <c r="S246" s="7"/>
-      <c r="T246" s="7"/>
-      <c r="U246" s="7"/>
-      <c r="V246" s="7"/>
-      <c r="W246" s="7"/>
-      <c r="X246" s="7"/>
-      <c r="Y246" s="7"/>
-      <c r="Z246" s="7"/>
-      <c r="AA246" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="247">
+      <c r="R246" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="S246" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="T246" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="U246" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="V246" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="W246" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="X246" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y246" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z246" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA246" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="247">
       <c r="C247" s="7" t="n">
         <v>2</v>
       </c>
@@ -12029,7 +12052,7 @@
         <v>85</v>
       </c>
       <c r="E247" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F247" s="7" t="s">
         <v>35</v>
@@ -12044,13 +12067,13 @@
         <v>27</v>
       </c>
       <c r="J247" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K247" s="7" t="s">
         <v>24</v>
       </c>
       <c r="L247" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M247" s="7" t="s">
         <v>16</v>
@@ -12064,18 +12087,38 @@
       <c r="Q247" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="R247" s="7"/>
-      <c r="S247" s="7"/>
-      <c r="T247" s="7"/>
-      <c r="U247" s="7"/>
-      <c r="V247" s="7"/>
-      <c r="W247" s="7"/>
-      <c r="X247" s="7"/>
-      <c r="Y247" s="7"/>
-      <c r="Z247" s="7"/>
-      <c r="AA247" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="248">
+      <c r="R247" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S247" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="T247" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U247" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="V247" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W247" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X247" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y247" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z247" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA247" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="248">
       <c r="C248" s="7" t="n">
         <v>3</v>
       </c>
@@ -12086,28 +12129,28 @@
         <v>49</v>
       </c>
       <c r="F248" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G248" s="7" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="H248" s="7" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="I248" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J248" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K248" s="7" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="L248" s="7" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="M248" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="N248" s="7" t="s">
         <v>35</v>
@@ -12118,16 +12161,36 @@
       <c r="Q248" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="R248" s="7"/>
-      <c r="S248" s="7"/>
-      <c r="T248" s="7"/>
-      <c r="U248" s="7"/>
-      <c r="V248" s="7"/>
-      <c r="W248" s="7"/>
-      <c r="X248" s="7"/>
-      <c r="Y248" s="7"/>
-      <c r="Z248" s="7"/>
-      <c r="AA248" s="7"/>
+      <c r="R248" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="S248" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T248" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="U248" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="V248" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="W248" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X248" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y248" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z248" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA248" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="249">
       <c r="C249" s="7" t="n">
@@ -12137,31 +12200,31 @@
         <v>88</v>
       </c>
       <c r="E249" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F249" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G249" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F249" s="7" t="s">
+      <c r="H249" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G249" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H249" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="I249" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J249" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K249" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J249" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K249" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="L249" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M249" s="7" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="N249" s="7" t="s">
         <v>25</v>
@@ -12172,34 +12235,74 @@
       <c r="Q249" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="R249" s="7"/>
-      <c r="S249" s="7"/>
-      <c r="T249" s="7"/>
-      <c r="U249" s="7"/>
-      <c r="V249" s="7"/>
-      <c r="W249" s="7"/>
-      <c r="X249" s="7"/>
-      <c r="Y249" s="7"/>
-      <c r="Z249" s="7"/>
-      <c r="AA249" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="250">
+      <c r="R249" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S249" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T249" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U249" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V249" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="W249" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="X249" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y249" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z249" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA249" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="250">
       <c r="C250" s="7" t="n">
         <v>5</v>
       </c>
       <c r="D250" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E250" s="7"/>
-      <c r="F250" s="7"/>
-      <c r="G250" s="7"/>
-      <c r="H250" s="7"/>
-      <c r="I250" s="7"/>
-      <c r="J250" s="7"/>
-      <c r="K250" s="7"/>
-      <c r="L250" s="7"/>
-      <c r="M250" s="7"/>
-      <c r="N250" s="7"/>
+      <c r="E250" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F250" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G250" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H250" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I250" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J250" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K250" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L250" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M250" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="N250" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="P250" s="7" t="n">
         <v>5</v>
       </c>
@@ -12217,23 +12320,43 @@
       <c r="Z250" s="7"/>
       <c r="AA250" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="251">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="251">
       <c r="C251" s="7" t="n">
         <v>6</v>
       </c>
       <c r="D251" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E251" s="7"/>
-      <c r="F251" s="7"/>
-      <c r="G251" s="7"/>
-      <c r="H251" s="7"/>
-      <c r="I251" s="7"/>
-      <c r="J251" s="7"/>
-      <c r="K251" s="7"/>
-      <c r="L251" s="7"/>
-      <c r="M251" s="7"/>
-      <c r="N251" s="7"/>
+      <c r="E251" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F251" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G251" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H251" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I251" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J251" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K251" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L251" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M251" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N251" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="P251" s="7" t="n">
         <v>6</v>
       </c>
@@ -12258,16 +12381,36 @@
       <c r="D252" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E252" s="7"/>
-      <c r="F252" s="7"/>
-      <c r="G252" s="7"/>
-      <c r="H252" s="7"/>
-      <c r="I252" s="7"/>
-      <c r="J252" s="7"/>
-      <c r="K252" s="7"/>
-      <c r="L252" s="7"/>
-      <c r="M252" s="7"/>
-      <c r="N252" s="7"/>
+      <c r="E252" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F252" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G252" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H252" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I252" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J252" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K252" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L252" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M252" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="N252" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="P252" s="7" t="n">
         <v>7</v>
       </c>
@@ -12292,16 +12435,36 @@
       <c r="D253" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E253" s="7"/>
-      <c r="F253" s="7"/>
-      <c r="G253" s="7"/>
-      <c r="H253" s="7"/>
-      <c r="I253" s="7"/>
-      <c r="J253" s="7"/>
-      <c r="K253" s="7"/>
-      <c r="L253" s="7"/>
-      <c r="M253" s="7"/>
-      <c r="N253" s="7"/>
+      <c r="E253" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F253" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G253" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H253" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I253" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J253" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K253" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L253" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M253" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="N253" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="P253" s="7" t="n">
         <v>8</v>
       </c>
@@ -12353,23 +12516,43 @@
       <c r="Z254" s="7"/>
       <c r="AA254" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="255">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="255">
       <c r="C255" s="7" t="n">
         <v>10</v>
       </c>
       <c r="D255" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E255" s="7"/>
-      <c r="F255" s="7"/>
-      <c r="G255" s="7"/>
-      <c r="H255" s="7"/>
-      <c r="I255" s="7"/>
-      <c r="J255" s="7"/>
-      <c r="K255" s="7"/>
-      <c r="L255" s="7"/>
-      <c r="M255" s="7"/>
-      <c r="N255" s="7"/>
+      <c r="E255" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F255" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G255" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H255" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I255" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J255" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K255" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L255" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M255" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N255" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="P255" s="7" t="n">
         <v>10</v>
       </c>
@@ -12387,23 +12570,43 @@
       <c r="Z255" s="7"/>
       <c r="AA255" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="256">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="256">
       <c r="C256" s="7" t="n">
         <v>11</v>
       </c>
       <c r="D256" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E256" s="7"/>
-      <c r="F256" s="7"/>
-      <c r="G256" s="7"/>
-      <c r="H256" s="7"/>
-      <c r="I256" s="7"/>
-      <c r="J256" s="7"/>
-      <c r="K256" s="7"/>
-      <c r="L256" s="7"/>
-      <c r="M256" s="7"/>
-      <c r="N256" s="7"/>
+      <c r="E256" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F256" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G256" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H256" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I256" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J256" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K256" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L256" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M256" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N256" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="P256" s="7" t="n">
         <v>11</v>
       </c>
@@ -12421,23 +12624,43 @@
       <c r="Z256" s="7"/>
       <c r="AA256" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="257">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="257">
       <c r="C257" s="7" t="n">
         <v>12</v>
       </c>
       <c r="D257" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E257" s="7"/>
-      <c r="F257" s="7"/>
-      <c r="G257" s="7"/>
-      <c r="H257" s="7"/>
-      <c r="I257" s="7"/>
-      <c r="J257" s="7"/>
-      <c r="K257" s="7"/>
-      <c r="L257" s="7"/>
-      <c r="M257" s="7"/>
-      <c r="N257" s="7"/>
+      <c r="E257" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F257" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G257" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H257" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I257" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J257" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K257" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L257" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M257" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="N257" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="P257" s="7" t="n">
         <v>12</v>
       </c>
@@ -12455,23 +12678,43 @@
       <c r="Z257" s="7"/>
       <c r="AA257" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="258">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="258">
       <c r="C258" s="7" t="n">
         <v>13</v>
       </c>
       <c r="D258" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E258" s="7"/>
-      <c r="F258" s="7"/>
-      <c r="G258" s="7"/>
-      <c r="H258" s="7"/>
-      <c r="I258" s="7"/>
-      <c r="J258" s="7"/>
-      <c r="K258" s="7"/>
-      <c r="L258" s="7"/>
-      <c r="M258" s="7"/>
-      <c r="N258" s="7"/>
+      <c r="E258" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F258" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G258" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H258" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I258" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J258" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K258" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L258" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M258" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="N258" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="P258" s="7" t="n">
         <v>13</v>
       </c>

</xml_diff>